<commit_message>
Modified Files to initiate print
</commit_message>
<xml_diff>
--- a/controller/rcpt/Rcpt_Template.xlsx
+++ b/controller/rcpt/Rcpt_Template.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
   <si>
     <t>OMM MAA TRADERS</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>For OMM MAA TRADERS</t>
+  </si>
+  <si>
+    <t>=spellNumber(H24)</t>
   </si>
 </sst>
 </file>
@@ -142,18 +145,13 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="\`\ #,##0.00"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -439,348 +437,349 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="12" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="13" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="10" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="13" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="14" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1294,10 +1293,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1305,439 +1305,446 @@
     <col min="3" max="3" width="11.5703125" customWidth="1"/>
     <col min="4" max="4" width="16.42578125" customWidth="1"/>
     <col min="8" max="8" width="15.28515625" customWidth="1"/>
+    <col min="11" max="11" width="35.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="104" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="3" t="s">
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
+      <c r="F1" s="106" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="4" t="s">
+      <c r="G1" s="106"/>
+      <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="7" t="s">
+      <c r="B2" s="108"/>
+      <c r="C2" s="108"/>
+      <c r="D2" s="108"/>
+      <c r="E2" s="108"/>
+      <c r="F2" s="109" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="8"/>
-      <c r="H2" s="9" t="s">
+      <c r="G2" s="110"/>
+      <c r="H2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="107" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="7" t="s">
+      <c r="B3" s="108"/>
+      <c r="C3" s="108"/>
+      <c r="D3" s="108"/>
+      <c r="E3" s="108"/>
+      <c r="F3" s="109" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="8"/>
-      <c r="H3" s="9" t="s">
+      <c r="G3" s="110"/>
+      <c r="H3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="111" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="13"/>
+      <c r="B4" s="112"/>
+      <c r="C4" s="112"/>
+      <c r="D4" s="112"/>
+      <c r="E4" s="112"/>
+      <c r="F4" s="113"/>
+      <c r="G4" s="113"/>
+      <c r="H4" s="3"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="104" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="16"/>
+      <c r="B5" s="105"/>
+      <c r="C5" s="105"/>
+      <c r="D5" s="105"/>
+      <c r="E5" s="105"/>
+      <c r="F5" s="114"/>
+      <c r="G5" s="121"/>
+      <c r="H5" s="122"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="17"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="20" t="s">
+      <c r="A6" s="115"/>
+      <c r="B6" s="116"/>
+      <c r="C6" s="116"/>
+      <c r="D6" s="116"/>
+      <c r="E6" s="116"/>
+      <c r="F6" s="117"/>
+      <c r="G6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="26">
+      <c r="H6" s="5">
         <v>21392901248</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="21"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="25"/>
+      <c r="A7" s="118"/>
+      <c r="B7" s="119"/>
+      <c r="C7" s="119"/>
+      <c r="D7" s="119"/>
+      <c r="E7" s="119"/>
+      <c r="F7" s="120"/>
+      <c r="G7" s="123"/>
+      <c r="H7" s="124"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="99" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="30" t="s">
+      <c r="B8" s="100"/>
+      <c r="C8" s="101"/>
+      <c r="D8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="31">
+      <c r="E8" s="102">
         <v>1</v>
       </c>
-      <c r="F8" s="32"/>
-      <c r="G8" s="33" t="s">
+      <c r="F8" s="103"/>
+      <c r="G8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="34">
+      <c r="H8" s="8">
         <v>40684</v>
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="56"/>
-      <c r="B9" s="57"/>
-      <c r="C9" s="58"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="38"/>
+      <c r="A9" s="74"/>
+      <c r="B9" s="75"/>
+      <c r="C9" s="76"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="96"/>
+      <c r="F9" s="96"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="11"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="56"/>
-      <c r="B10" s="57"/>
-      <c r="C10" s="58"/>
-      <c r="D10" s="59" t="s">
+      <c r="A10" s="74"/>
+      <c r="B10" s="75"/>
+      <c r="C10" s="76"/>
+      <c r="D10" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="41"/>
+      <c r="E10" s="97"/>
+      <c r="F10" s="97"/>
+      <c r="G10" s="97"/>
+      <c r="H10" s="98"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="56"/>
-      <c r="B11" s="57"/>
-      <c r="C11" s="58"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="43"/>
+      <c r="A11" s="74"/>
+      <c r="B11" s="75"/>
+      <c r="C11" s="76"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="93"/>
+      <c r="F11" s="93"/>
+      <c r="G11" s="93"/>
+      <c r="H11" s="94"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="56"/>
-      <c r="B12" s="57"/>
-      <c r="C12" s="58"/>
-      <c r="D12" s="60" t="s">
+      <c r="A12" s="74"/>
+      <c r="B12" s="75"/>
+      <c r="C12" s="76"/>
+      <c r="D12" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="44"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="44"/>
-      <c r="H12" s="45"/>
+      <c r="E12" s="91"/>
+      <c r="F12" s="91"/>
+      <c r="G12" s="91"/>
+      <c r="H12" s="92"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="46" t="s">
+      <c r="A13" s="82" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="47"/>
-      <c r="C13" s="48"/>
-      <c r="D13" s="60"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="42"/>
-      <c r="H13" s="43"/>
+      <c r="B13" s="83"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="93"/>
+      <c r="F13" s="93"/>
+      <c r="G13" s="93"/>
+      <c r="H13" s="94"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="49" t="s">
+      <c r="A14" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="50"/>
-      <c r="C14" s="51"/>
-      <c r="D14" s="61" t="s">
+      <c r="B14" s="73"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="E14" s="53"/>
-      <c r="F14" s="53"/>
-      <c r="G14" s="54" t="s">
+      <c r="E14" s="95"/>
+      <c r="F14" s="95"/>
+      <c r="G14" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="55">
+      <c r="H14" s="17">
         <v>40684</v>
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="62" t="s">
+      <c r="A15" s="84" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="63"/>
-      <c r="C15" s="64"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="65"/>
-      <c r="F15" s="65"/>
-      <c r="G15" s="65"/>
-      <c r="H15" s="64"/>
+      <c r="B15" s="85"/>
+      <c r="C15" s="86"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="87"/>
+      <c r="F15" s="87"/>
+      <c r="G15" s="87"/>
+      <c r="H15" s="86"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="56"/>
-      <c r="B16" s="57"/>
-      <c r="C16" s="58"/>
-      <c r="D16" s="66" t="s">
+      <c r="A16" s="74"/>
+      <c r="B16" s="75"/>
+      <c r="C16" s="76"/>
+      <c r="D16" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="67"/>
-      <c r="F16" s="67"/>
-      <c r="G16" s="67"/>
-      <c r="H16" s="68"/>
+      <c r="E16" s="88"/>
+      <c r="F16" s="88"/>
+      <c r="G16" s="88"/>
+      <c r="H16" s="89"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="56"/>
-      <c r="B17" s="57"/>
-      <c r="C17" s="58"/>
-      <c r="D17" s="66"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="47"/>
-      <c r="H17" s="69"/>
+      <c r="A17" s="74"/>
+      <c r="B17" s="75"/>
+      <c r="C17" s="76"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="83"/>
+      <c r="F17" s="83"/>
+      <c r="G17" s="83"/>
+      <c r="H17" s="90"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="56"/>
-      <c r="B18" s="57"/>
-      <c r="C18" s="58"/>
-      <c r="D18" s="66" t="s">
+      <c r="A18" s="74"/>
+      <c r="B18" s="75"/>
+      <c r="C18" s="76"/>
+      <c r="D18" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="72"/>
-      <c r="F18" s="72"/>
-      <c r="G18" s="72"/>
-      <c r="H18" s="73"/>
+      <c r="E18" s="77"/>
+      <c r="F18" s="77"/>
+      <c r="G18" s="77"/>
+      <c r="H18" s="78"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="56"/>
-      <c r="B19" s="57"/>
-      <c r="C19" s="58"/>
-      <c r="D19" s="66"/>
-      <c r="E19" s="72"/>
-      <c r="F19" s="72"/>
-      <c r="G19" s="72"/>
-      <c r="H19" s="73"/>
+      <c r="A19" s="74"/>
+      <c r="B19" s="75"/>
+      <c r="C19" s="76"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="77"/>
+      <c r="F19" s="77"/>
+      <c r="G19" s="77"/>
+      <c r="H19" s="78"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="46" t="s">
+      <c r="A20" s="82" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="47"/>
-      <c r="C20" s="70"/>
-      <c r="D20" s="66"/>
-      <c r="E20" s="72"/>
-      <c r="F20" s="72"/>
-      <c r="G20" s="72"/>
-      <c r="H20" s="73"/>
+      <c r="B20" s="83"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="77"/>
+      <c r="F20" s="77"/>
+      <c r="G20" s="77"/>
+      <c r="H20" s="78"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="49" t="s">
+      <c r="A21" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="50"/>
-      <c r="C21" s="71"/>
-      <c r="D21" s="52"/>
-      <c r="E21" s="74"/>
-      <c r="F21" s="74"/>
-      <c r="G21" s="74"/>
-      <c r="H21" s="75"/>
+      <c r="B21" s="73"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="79"/>
+      <c r="F21" s="79"/>
+      <c r="G21" s="79"/>
+      <c r="H21" s="80"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="77" t="s">
+      <c r="A22" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="78" t="s">
+      <c r="B22" s="81" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="78"/>
-      <c r="D22" s="77" t="s">
+      <c r="C22" s="81"/>
+      <c r="D22" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="E22" s="77" t="s">
+      <c r="E22" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="F22" s="77" t="s">
+      <c r="F22" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="G22" s="77" t="s">
+      <c r="G22" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="H22" s="77" t="s">
+      <c r="H22" s="24" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="B23" s="76"/>
-      <c r="C23" s="76"/>
+      <c r="A23" s="31"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="31"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="79"/>
-      <c r="B24" s="80"/>
-      <c r="C24" s="81"/>
-      <c r="D24" s="82" t="s">
+      <c r="A24" s="25"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="E24" s="83"/>
-      <c r="F24" s="81"/>
-      <c r="G24" s="81"/>
-      <c r="H24" s="84"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="30">
+        <v>111</v>
+      </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="85" t="str">
-        <f>SpellNo3</f>
-        <v>Rupees Three Hundred Ninety-Nine and Paise Fifty Only</v>
-      </c>
-      <c r="B25" s="86"/>
-      <c r="C25" s="87"/>
-      <c r="D25" s="88" t="s">
+      <c r="A25" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="46"/>
+      <c r="C25" s="47"/>
+      <c r="D25" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="E25" s="89"/>
-      <c r="F25" s="89"/>
-      <c r="G25" s="89"/>
-      <c r="H25" s="90"/>
+      <c r="E25" s="52"/>
+      <c r="F25" s="52"/>
+      <c r="G25" s="52"/>
+      <c r="H25" s="53"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="91"/>
-      <c r="B26" s="92"/>
-      <c r="C26" s="93"/>
-      <c r="D26" s="94"/>
-      <c r="E26" s="95"/>
-      <c r="F26" s="95"/>
-      <c r="G26" s="95"/>
-      <c r="H26" s="96"/>
+      <c r="A26" s="48"/>
+      <c r="B26" s="49"/>
+      <c r="C26" s="50"/>
+      <c r="D26" s="54"/>
+      <c r="E26" s="55"/>
+      <c r="F26" s="55"/>
+      <c r="G26" s="55"/>
+      <c r="H26" s="56"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="97" t="s">
+      <c r="A27" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="98"/>
-      <c r="C27" s="99"/>
-      <c r="D27" s="94"/>
-      <c r="E27" s="95"/>
-      <c r="F27" s="95"/>
-      <c r="G27" s="95"/>
-      <c r="H27" s="96"/>
+      <c r="B27" s="61"/>
+      <c r="C27" s="62"/>
+      <c r="D27" s="54"/>
+      <c r="E27" s="55"/>
+      <c r="F27" s="55"/>
+      <c r="G27" s="55"/>
+      <c r="H27" s="56"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="100"/>
-      <c r="B28" s="101"/>
-      <c r="C28" s="102"/>
-      <c r="D28" s="103"/>
-      <c r="E28" s="104"/>
-      <c r="F28" s="104"/>
-      <c r="G28" s="104"/>
-      <c r="H28" s="105"/>
+      <c r="A28" s="63"/>
+      <c r="B28" s="64"/>
+      <c r="C28" s="65"/>
+      <c r="D28" s="57"/>
+      <c r="E28" s="58"/>
+      <c r="F28" s="58"/>
+      <c r="G28" s="58"/>
+      <c r="H28" s="59"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="106" t="s">
+      <c r="A29" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="107"/>
-      <c r="C29" s="108"/>
-      <c r="D29" s="109" t="s">
+      <c r="B29" s="67"/>
+      <c r="C29" s="68"/>
+      <c r="D29" s="69" t="s">
         <v>36</v>
       </c>
-      <c r="E29" s="110"/>
-      <c r="F29" s="110"/>
-      <c r="G29" s="110"/>
-      <c r="H29" s="111"/>
+      <c r="E29" s="70"/>
+      <c r="F29" s="70"/>
+      <c r="G29" s="70"/>
+      <c r="H29" s="71"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="112" t="s">
+      <c r="A30" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="B30" s="113"/>
-      <c r="C30" s="114"/>
-      <c r="D30" s="115"/>
-      <c r="E30" s="116"/>
-      <c r="F30" s="116"/>
-      <c r="G30" s="116"/>
-      <c r="H30" s="117"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="34"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="40"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="112"/>
-      <c r="B31" s="113"/>
-      <c r="C31" s="114"/>
-      <c r="D31" s="115"/>
-      <c r="E31" s="116"/>
-      <c r="F31" s="116"/>
-      <c r="G31" s="116"/>
-      <c r="H31" s="117"/>
+      <c r="A31" s="32"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="39"/>
+      <c r="F31" s="39"/>
+      <c r="G31" s="39"/>
+      <c r="H31" s="40"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="112"/>
-      <c r="B32" s="113"/>
-      <c r="C32" s="114"/>
-      <c r="D32" s="115"/>
-      <c r="E32" s="116"/>
-      <c r="F32" s="116"/>
-      <c r="G32" s="116"/>
-      <c r="H32" s="117"/>
+      <c r="A32" s="32"/>
+      <c r="B32" s="33"/>
+      <c r="C32" s="34"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="39"/>
+      <c r="F32" s="39"/>
+      <c r="G32" s="39"/>
+      <c r="H32" s="40"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="118"/>
-      <c r="B33" s="119"/>
-      <c r="C33" s="120"/>
-      <c r="D33" s="121" t="s">
+      <c r="A33" s="35"/>
+      <c r="B33" s="36"/>
+      <c r="C33" s="37"/>
+      <c r="D33" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="E33" s="122"/>
-      <c r="F33" s="122"/>
-      <c r="G33" s="122"/>
-      <c r="H33" s="123"/>
+      <c r="E33" s="42"/>
+      <c r="F33" s="42"/>
+      <c r="G33" s="42"/>
+      <c r="H33" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A30:C33"/>
-    <mergeCell ref="D30:H32"/>
-    <mergeCell ref="D33:H33"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="A25:C26"/>
-    <mergeCell ref="D25:H28"/>
-    <mergeCell ref="A27:C28"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="D29:H29"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A16:C19"/>
-    <mergeCell ref="E18:H21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="A5:F7"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G7:H7"/>
     <mergeCell ref="A15:C15"/>
     <mergeCell ref="E15:H15"/>
     <mergeCell ref="E16:H16"/>
@@ -1751,19 +1758,20 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:H10"/>
     <mergeCell ref="E11:H11"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="A5:F7"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A16:C19"/>
+    <mergeCell ref="E18:H21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A30:C33"/>
+    <mergeCell ref="D30:H32"/>
+    <mergeCell ref="D33:H33"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="A25:C26"/>
+    <mergeCell ref="D25:H28"/>
+    <mergeCell ref="A27:C28"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="D29:H29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>